<commit_message>
added the possibility of using mistral
</commit_message>
<xml_diff>
--- a/Adresses_test_correct.xlsx
+++ b/Adresses_test_correct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkassis\Documents\GitHub\SBS-intern-AI-adress-treatment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B567F6C-8FF7-4DD3-870F-FD0C64E45D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22761BBB-F046-4207-ACAA-E163145B984A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12741,8 +12741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="F12" zoomScale="95" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12760,7 +12760,7 @@
     <col min="12" max="12" width="80.21875" customWidth="1"/>
     <col min="13" max="13" width="32" customWidth="1"/>
     <col min="14" max="14" width="22.5546875" customWidth="1"/>
-    <col min="15" max="15" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="39.33203125" customWidth="1"/>
     <col min="16" max="16" width="34.21875" customWidth="1"/>
     <col min="17" max="17" width="16.77734375" customWidth="1"/>
   </cols>

</xml_diff>